<commit_message>
upload amplicon and growth data for project GEP00013; fix code for loading project from script and for plotting growth
</commit_message>
<xml_diff>
--- a/data/GEP00013/GEP00013.xlsx
+++ b/data/GEP00013/GEP00013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29140" windowHeight="20380" tabRatio="736" activeTab="5"/>
+    <workbookView xWindow="36500" yWindow="0" windowWidth="29140" windowHeight="20380" tabRatio="736" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="10" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2745" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2745" uniqueCount="646">
   <si>
     <t>geid</t>
   </si>
@@ -2100,6 +2100,9 @@
   </si>
   <si>
     <t>CTGACTGGACCTCCTGCTCT</t>
+  </si>
+  <si>
+    <t>C6</t>
   </si>
 </sst>
 </file>
@@ -4315,8 +4318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -5455,7 +5458,7 @@
         <v>219</v>
       </c>
       <c r="B44" t="s">
-        <v>198</v>
+        <v>645</v>
       </c>
       <c r="C44" t="s">
         <v>154</v>
@@ -7915,7 +7918,7 @@
         <v>258</v>
       </c>
       <c r="B140" t="s">
-        <v>198</v>
+        <v>645</v>
       </c>
       <c r="C140" t="s">
         <v>154</v>
@@ -9389,7 +9392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G193"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F168" sqref="F168"/>
     </sheetView>
   </sheetViews>

</xml_diff>